<commit_message>
modified code overview file
</commit_message>
<xml_diff>
--- a/code_overview_fresh_vs_frozen_comparison.xlsx
+++ b/code_overview_fresh_vs_frozen_comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="143">
   <si>
     <t xml:space="preserve">File name</t>
   </si>
@@ -73,109 +73,382 @@
     <t xml:space="preserve">cell_type_annotation/reannotate_uveal_melanoma_tcells.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Annotate T cells in uveal melanoma metastatic samples more finely</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated rds file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated rds file of T-cells with finer T cell annotation</t>
+  </si>
+  <si>
     <t xml:space="preserve">cell_type_annotation/reannotate_uveal_melanoma_tcells_nk.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Check whether two clusters in integrated uveal melanoma metastatic T-cells data are NK cells, by reclustering them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">cell_type_annotation/reannotate_uveal_melanoma_tcells_vln_plots.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Plotting violin plots of T cell exhaustion signatures in integrated uveal melanoma metastatic T cell data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Violin plots of T-cell exhaustion signature strengths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell_type_annotation/reannotate_ribas_melanoma_tcells.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annotate T cells in cutaneous melanoma sequential samples more finely</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual sample rds files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated rds file with finer T cell annotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell_type_annotation/reannotate_BI5_and_uveal_primary_tcells.R</t>
+  </si>
+  <si>
     <t xml:space="preserve">correlation_with_wgs/correlate_wgs_and_infercnv.R</t>
   </si>
   <si>
-    <t xml:space="preserve">correlation_with_wgs/correlation_with_wgs.R</t>
-  </si>
-  <si>
     <t xml:space="preserve">geo_submission/geo_submission.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Print out csv files of count matrices for single-nucleus and single-cell sequencing data across all datasets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Csv files of counts for each sample</t>
+  </si>
+  <si>
     <t xml:space="preserve">geo_submission/mbpm_puckdata_printout_info_for_geo_fresh_vs_frozen_comparison.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Print out csv files of count matrices for spatial sequencing data for sequential cutaneous melanoma samples</t>
+  </si>
+  <si>
     <t xml:space="preserve">infercnv_analyses/make_infercnv_plots2.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Make heatmap plots of infercnv results for all datasets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual sample rds files containing infercnv results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heatmaps of infercnv results for each sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infercnv_analyses/fresh_vs_frozen_infercnv_comparison.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infercnv_analyses/r310_infercnv_and_resistance_sig.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infercnv_analyses/r310_rename_segfiles.R</t>
+  </si>
+  <si>
     <t xml:space="preserve">initial_processing/Seurat_cellbender_fresh_vs_frozen_comparison.R</t>
   </si>
   <si>
-    <t xml:space="preserve">initial_processing/Seurat_cellbender_fresh_vs_frozen_comparison_last_four.R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">initial_processing/Seurat_cellbender_fresh_vs_frozen_comparison_slyper_pipeline.R</t>
+    <t xml:space="preserve">Creation of Seurat object from Cellbender output, and doublet and QC thresholding, for cutaneous melanoma, uveal melanoma primary, and nsclc samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cellbender output (filtered .h5 files) for each individual samples</t>
   </si>
   <si>
     <t xml:space="preserve">initial_processing/Seurat_cellbender_ribas_melanoma.R</t>
   </si>
   <si>
-    <t xml:space="preserve">initial_processing/Seurat_cellbender_ribas_on_titrate_thresh.R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">initial_processing/Seurat_cellbender_uveal_melanoma.R</t>
+    <t xml:space="preserve">Creation of Seurat object from Cellbender output, and doublet and QC thresholding, for cutaneous melanoma samples under pembrolizumab treatment</t>
   </si>
   <si>
     <t xml:space="preserve">initial_processing/Seurat_cellbender_uveal_melanoma_new_samples.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Creation of Seurat object from Cellbender output, and doublet and QC thresholding, for uveal melanoma liver metastasis samples</t>
+  </si>
+  <si>
     <t xml:space="preserve">initial_processing/Seurat_integrate_fresh_vs_frozen_comparison.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Seurat integration of cutaneous melanoma, uveal melanoma primary, and nsclc samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated rds files for each dataset</t>
+  </si>
+  <si>
     <t xml:space="preserve">initial_processing/Seurat_integrate_uveal_melanoma_new_samples.R</t>
   </si>
   <si>
-    <t xml:space="preserve">initial_processing/slyper_pipeline_downsampling.R</t>
+    <t xml:space="preserve">Seurat integration of uveal melanoma liver metastasis samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated rds file of uveal melanoma liver metastasis data</t>
   </si>
   <si>
     <t xml:space="preserve">QC_metrics/QC_vln_plots.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Plotting violin plots of quality metrics for all datasets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Violin plots of QC metrics for each dataset</t>
+  </si>
+  <si>
     <t xml:space="preserve">QC_metrics/load_stress_sigs.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Load lists of stress signature genes to calculate strength of these signatures across all datasets</t>
+  </si>
+  <si>
     <t xml:space="preserve">QC_metrics/rename_sample_IDs.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Rename sample IDs in rds objects across all datasets to human-readable format for plotting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated rds files for each dataset with sample names renamed to human-readable format</t>
+  </si>
+  <si>
     <t xml:space="preserve">sampling_to_uniform_saturation/sampling_to_uniform_saturation.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Downsample UMI counts in cutaneous melanoma and NSCLC datasets, across both slyper and non-slyper protocols, to obtain comparable UMI counts across samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtered .h5 files with downsampled read counts for each sample</t>
+  </si>
+  <si>
     <t xml:space="preserve">sampling_to_uniform_saturation/sampling_to_uniform_saturation_vlnplots.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Plotting violin plots of quality metrics for cutaneous melanoma and NSCLC datasets, using data downsampled to obtain comparable UMI counts across samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated rds files for each dataset, with downsampled reads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Violin plots of QC metrics for each dataset, using downsampled data</t>
+  </si>
+  <si>
     <t xml:space="preserve">scenic_analyses/r310_scenic_and_infercnv.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Determine regulators from scenic analysis that are differentially expressed in clone 2 of sequential cutaneous melanoma dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Csv files containing AUCell results from scenic for each sample, individual sample rds files, and rds files containing infercnv results for each sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dotplot showing all scenic regulators that are differentially between clone 2 and non-clone 2 cells across all timepoints</t>
+  </si>
+  <si>
     <t xml:space="preserve">scenic_analyses/scenic_prep.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Print out csv files of count matrices for sequential cutaneous melanoma samples</t>
+  </si>
+  <si>
     <t xml:space="preserve">scenic_analyses/scenic_run.py</t>
   </si>
   <si>
-    <t xml:space="preserve">scenic_analyses/splitChromosomes.py</t>
+    <t xml:space="preserve">Run scenic for each sample in sequential cutaneous melanoma dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Csv files containing AUCell results from scenic for each sample</t>
   </si>
   <si>
     <t xml:space="preserve">TCR_analyses/TCR_circos.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Create circos plots showing overlap in TCR clonotypes between fresh and frozen samples in cutaneous melanoma, NSCLC, and uveal primary datasets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csv files containing clonotype annotations for each sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circos plots showing clonotype overlap among samples in each dataset</t>
+  </si>
+  <si>
     <t xml:space="preserve">TCR_analyses/TCR_clonality_umaps.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Create umaps of T cells with TCR clonality plotted in different colors according to frequency, for cutaneous melanoma, uveal melanoma primary, uveal melanoma metastasis, and sequential cutaneous melanoma samples under pembrolizumab therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umaps of T-cells for each dataset, with TCR clonality plotted in different colors by frequency</t>
+  </si>
+  <si>
     <t xml:space="preserve">TCR_analyses/assign_TCR_clonality.R</t>
   </si>
   <si>
-    <t xml:space="preserve">trajectory_analysis/rglscript_user.R</t>
+    <t xml:space="preserve">Assign TCR clonality information to T cells to rds files for a particular dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csv files containing clonotype frequencies for each sample, and integrated rds files for each dataset </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated rds files for each dataset, with clonality information added</t>
   </si>
   <si>
     <t xml:space="preserve">trajectory_analysis/t_cell_destiny.R</t>
   </si>
   <si>
-    <t xml:space="preserve">wes_analyses/convertIntervalListToBed.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wes_analyses/convertb37tohg19vcf.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wes_analyses/lightenCollectReadCountsTSV.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wes_analyses/wes_pipeline.R</t>
+    <t xml:space="preserve">Perform diffusion analysis for T-cells from cutaneous melanoma samples under therapy and uveal melanoma metastatic samples, and plot signatures of T-cell activation and exhaustion on diffusion maps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated rds files for T-cells from each dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diffusion maps of T-cells from each dataset, with signature strength plotted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wes_analyses/whole_exome_pipeline.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download reference files for whole exome analysis, and whole exome sequencing fastq files for cutaneous melanoma sequential therapy samples, map fastq files to generate bam files, and run controlFREEC with these inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whole exome sequencing fastq files for each sample, hg19 fastq reference sequence, and fastq files of each chromosome in hg19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seg files containing copy number results for each sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wes_analyses/splitChromosomes.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Split a fastq file containing entire hg19 sequence into fastq files for each chromosome, for use by controlFREEC program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fastq file containing entire hg19 sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fastq files containing sequences of each chromosome in hg19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">final_Tcell_comparisons.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granular annotation of T-cells and comparison of T-cell dynamics across metastatic niches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anndata objects, gene signatures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See Figures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figures 4d,e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slideseq_starfysh_tutorial_on_later.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run Starfysh on slideseq data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slideseq coordinates, counts, gene signatures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figures 3a,b; ED 6f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">final_um_analysis.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process and visualize uveal data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 4a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fresh_frozen_comparisons/final_scVI_correction_example.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply scVI correction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anndata object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Results from scVI batch correction as anndata object, UMAP coordinates, components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fresh_frozen_comparisons/final_Seurat_STACAS_example.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply Seurat and STACAS for batch correction; compute LISI scores; visualize all batch correction results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDS files containing data for each dataset; outputs from final_scVI_correction_example.ipynb; annotations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figures ED 3,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fresh_frozen_comparisons/final_splicing_fractions.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualize Velocyto results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocyto outputs; annotations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See Tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ED Table 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r310_analysis/final_analysis_r310.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster r310 data, visualize gene signatures, analyze clonal dynamics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anndata object; inferCNV outputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rnk files; See Figures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figures 2c-g; ED 7c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r310_analysis/final_gsea.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate plot for visualizing GSEA results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rnk files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure ED 7d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r310_analysis/final_r310_all_cells_process.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualize cells in r310 and match to annotations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anndata object; annotations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processed anndata for r310; See Figures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 2A</t>
   </si>
 </sst>
 </file>
@@ -185,11 +458,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -213,6 +487,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -257,7 +536,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -268,6 +547,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -287,13 +574,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
   </cols>
@@ -364,180 +651,551 @@
       <c r="A5" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
+        <v>35</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>37</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>33</v>
+        <v>57</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>34</v>
+        <v>60</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>35</v>
+        <v>62</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>65</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>37</v>
+        <v>68</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>38</v>
+        <v>72</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>39</v>
+        <v>76</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>40</v>
+        <v>78</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>41</v>
+        <v>81</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>42</v>
+        <v>85</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>43</v>
+        <v>88</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>44</v>
+        <v>92</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>45</v>
+        <v>96</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>48</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>51</v>
+      <c r="A38" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified code_overview and README
</commit_message>
<xml_diff>
--- a/code_overview_fresh_vs_frozen_comparison.xlsx
+++ b/code_overview_fresh_vs_frozen_comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="168">
   <si>
     <t xml:space="preserve">File name</t>
   </si>
@@ -70,6 +70,9 @@
     <t xml:space="preserve">Barplots of cell type frequency, immune and non-immune simpson diversity, and malignant cell fraction across datasets</t>
   </si>
   <si>
+    <t xml:space="preserve">ED Figure5A-C</t>
+  </si>
+  <si>
     <t xml:space="preserve">cell_type_annotation/reannotate_uveal_melanoma_tcells.R</t>
   </si>
   <si>
@@ -118,6 +121,15 @@
     <t xml:space="preserve">correlation_with_wgs/correlate_wgs_and_infercnv.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Correlate average arm-level infercnv and whole-genome sequencing copy number alterations in uveal melanoma metastatic dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rds files containing single-cell data and infercnv data for each sample, and seg files with whole genome cnv information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 4C</t>
+  </si>
+  <si>
     <t xml:space="preserve">geo_submission/geo_submission.R</t>
   </si>
   <si>
@@ -136,7 +148,8 @@
     <t xml:space="preserve">infercnv_analyses/make_infercnv_plots2.R</t>
   </si>
   <si>
-    <t xml:space="preserve">Make heatmap plots of infercnv results for all datasets</t>
+    <t xml:space="preserve">Make heatmap plots of infercnv 
+results for all datasets</t>
   </si>
   <si>
     <t xml:space="preserve">Individual sample rds files containing infercnv results</t>
@@ -145,13 +158,31 @@
     <t xml:space="preserve">Heatmaps of infercnv results for each sample</t>
   </si>
   <si>
+    <t xml:space="preserve">Figure 2B, 4B left panel, ED Figure 9B, 9C lower panel</t>
+  </si>
+  <si>
     <t xml:space="preserve">infercnv_analyses/fresh_vs_frozen_infercnv_comparison.R</t>
   </si>
   <si>
+    <t xml:space="preserve">Correlate average arm-level infercnv copy numter alterations in fresh vs. Frozen samples in cutaneous melanoma, uveal primary, and NSCLC datasets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rds files containing infercnv data for each sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 1I</t>
+  </si>
+  <si>
     <t xml:space="preserve">infercnv_analyses/r310_infercnv_and_resistance_sig.R</t>
   </si>
   <si>
-    <t xml:space="preserve">infercnv_analyses/r310_rename_segfiles.R</t>
+    <t xml:space="preserve">Print heatmap of infercnv copy number changes, with histogram of immune resistance signature gene density overtop, for each sample in cutaneous melanoma sequential treatment dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rds files containing single-cell data and infercnv data for each sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ED Figure7F</t>
   </si>
   <si>
     <t xml:space="preserve">initial_processing/Seurat_cellbender_fresh_vs_frozen_comparison.R</t>
@@ -202,6 +233,9 @@
     <t xml:space="preserve">Violin plots of QC metrics for each dataset</t>
   </si>
   <si>
+    <t xml:space="preserve">Figure 1A-F, ED Figure 1A-D, ED Figure 6B-C, ED Figure 7A-B, ED Figure 8B</t>
+  </si>
+  <si>
     <t xml:space="preserve">QC_metrics/load_stress_sigs.R</t>
   </si>
   <si>
@@ -250,6 +284,9 @@
     <t xml:space="preserve">Dotplot showing all scenic regulators that are differentially between clone 2 and non-clone 2 cells across all timepoints</t>
   </si>
   <si>
+    <t xml:space="preserve">ED Figure7E, G</t>
+  </si>
+  <si>
     <t xml:space="preserve">scenic_analyses/scenic_prep.R</t>
   </si>
   <si>
@@ -277,6 +314,9 @@
     <t xml:space="preserve">Circos plots showing clonotype overlap among samples in each dataset</t>
   </si>
   <si>
+    <t xml:space="preserve">Figure 1G-H, Figure 2I</t>
+  </si>
+  <si>
     <t xml:space="preserve">TCR_analyses/TCR_clonality_umaps.R</t>
   </si>
   <si>
@@ -286,6 +326,9 @@
     <t xml:space="preserve">Umaps of T-cells for each dataset, with TCR clonality plotted in different colors by frequency</t>
   </si>
   <si>
+    <t xml:space="preserve">ED Figure 2A-B, ED Figure 6D-E</t>
+  </si>
+  <si>
     <t xml:space="preserve">TCR_analyses/assign_TCR_clonality.R</t>
   </si>
   <si>
@@ -310,6 +353,9 @@
     <t xml:space="preserve">Diffusion maps of T-cells from each dataset, with signature strength plotted</t>
   </si>
   <si>
+    <t xml:space="preserve">Figure 2H</t>
+  </si>
+  <si>
     <t xml:space="preserve">wes_analyses/whole_exome_pipeline.sh</t>
   </si>
   <si>
@@ -322,6 +368,9 @@
     <t xml:space="preserve">Seg files containing copy number results for each sample</t>
   </si>
   <si>
+    <t xml:space="preserve">ED Figure6H</t>
+  </si>
+  <si>
     <t xml:space="preserve">wes_analyses/splitChromosomes.py</t>
   </si>
   <si>
@@ -332,6 +381,33 @@
   </si>
   <si>
     <t xml:space="preserve">Fastq files containing sequences of each chromosome in hg19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial_analysis/rctd_mbpm_puckdata.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use RCTD pipeline to assign cell type identities to SlideSeq samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rds object containing single-nuclei reference data, rds files containing puck data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rds files containing rctd results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial_analysis/rctd_mbpm_puckdata_plot_cell_types_pub_quality.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot figures that show predicted cell types from RCTD across pucks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rds files containing individual sample data, and rctd inferred cell types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ED Figure 6G</t>
   </si>
   <si>
     <t xml:space="preserve">final_Tcell_comparisons.ipynb</t>
@@ -458,7 +534,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -490,8 +566,23 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -536,7 +627,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -549,12 +640,24 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -574,15 +677,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,559 +752,654 @@
       <c r="D4" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="E4" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>43</v>
+        <v>54</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>52</v>
+        <v>64</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>68</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>56</v>
+        <v>69</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>71</v>
+        <v>86</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>80</v>
+        <v>96</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>84</v>
+        <v>100</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>91</v>
+        <v>109</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>95</v>
+        <v>114</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" s="4"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E43" s="0" t="s">
+      <c r="D38" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B39" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C39" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="D44" s="4" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>142</v>
       </c>
+      <c r="C40" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>167</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A35" r:id="rId1" display="https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial"/>
+    <hyperlink ref="A36" r:id="rId2" display="https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added table information to code_overview
</commit_message>
<xml_diff>
--- a/code_overview_fresh_vs_frozen_comparison.xlsx
+++ b/code_overview_fresh_vs_frozen_comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="169">
   <si>
     <t xml:space="preserve">File name</t>
   </si>
@@ -236,6 +236,9 @@
     <t xml:space="preserve">Figure 1A-F, ED Figure 1A-D, ED Figure 6B-C, ED Figure 7A-B, ED Figure 8B</t>
   </si>
   <si>
+    <t xml:space="preserve">ED Table 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">QC_metrics/load_stress_sigs.R</t>
   </si>
   <si>
@@ -317,6 +320,9 @@
     <t xml:space="preserve">Figure 1G-H, Figure 2I</t>
   </si>
   <si>
+    <t xml:space="preserve">ED Table 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">TCR_analyses/TCR_clonality_umaps.R</t>
   </si>
   <si>
@@ -480,9 +486,6 @@
   </si>
   <si>
     <t xml:space="preserve">See Tables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ED Table 2</t>
   </si>
   <si>
     <t xml:space="preserve">r310_analysis/final_analysis_r310.ipynb</t>
@@ -679,11 +682,11 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.21"/>
@@ -1005,13 +1008,16 @@
       <c r="E21" s="0" t="s">
         <v>70</v>
       </c>
+      <c r="F21" s="0" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>23</v>
@@ -1022,69 +1028,69 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>63</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>29</v>
@@ -1095,130 +1101,133 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>63</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -1226,179 +1235,179 @@
     </row>
     <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="E38" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A35" r:id="rId1" display="https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial"/>
-    <hyperlink ref="A36" r:id="rId2" display="https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial"/>
+    <hyperlink ref="A35" r:id="rId1" display="https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial_analysis/rctd_mbpm_puckdata.R"/>
+    <hyperlink ref="A36" r:id="rId2" display="https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial_analysis/rctd_mbpm_puckdata_plot_cell_types_pub_quality.R"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added gini script for TCR analyses, updated scenic run script
</commit_message>
<xml_diff>
--- a/code_overview_fresh_vs_frozen_comparison.xlsx
+++ b/code_overview_fresh_vs_frozen_comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="173">
   <si>
     <t xml:space="preserve">File name</t>
   </si>
@@ -345,6 +345,18 @@
   </si>
   <si>
     <t xml:space="preserve">Integrated rds files for each dataset, with clonality information added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR_analyses/giniscript.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate Gini coefficients for TCR clonotype data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text files containing clonotype frequency data, from TCR_circos.R script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text files containing Gini TCR coefficients</t>
   </si>
   <si>
     <t xml:space="preserve">trajectory_analysis/t_cell_destiny.R</t>
@@ -680,13 +692,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.21"/>
@@ -1177,148 +1189,148 @@
       <c r="D32" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E32" s="0" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="C33" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="D33" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="E33" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="C34" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="D34" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="E34" s="0" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-    </row>
-    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="C36" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="D36" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" s="3" t="s">
+      <c r="E37" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="3"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>139</v>
       </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="E39" s="0" t="s">
+      <c r="C39" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B40" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="B40" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="C40" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>147</v>
       </c>
@@ -1329,13 +1341,10 @@
         <v>149</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E41" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>151</v>
       </c>
@@ -1346,14 +1355,13 @@
         <v>153</v>
       </c>
       <c r="D42" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="43" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>155</v>
       </c>
@@ -1366,28 +1374,29 @@
       <c r="D43" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>164</v>
       </c>
@@ -1398,16 +1407,33 @@
         <v>166</v>
       </c>
       <c r="D45" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="E45" s="3" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
         <v>168</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A35" r:id="rId1" display="https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial_analysis/rctd_mbpm_puckdata.R"/>
-    <hyperlink ref="A36" r:id="rId2" display="https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial_analysis/rctd_mbpm_puckdata_plot_cell_types_pub_quality.R"/>
+    <hyperlink ref="A36" r:id="rId1" display="https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial_analysis/rctd_mbpm_puckdata.R"/>
+    <hyperlink ref="A37" r:id="rId2" display="https://github.com/IzarLab/Melanoma_Brain_Metastasis/Spatial_analysis/rctd_mbpm_puckdata_plot_cell_types_pub_quality.R"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>